<commit_message>
update short report & actual.html
</commit_message>
<xml_diff>
--- a/public/Краткий отчет.xlsx
+++ b/public/Краткий отчет.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="356">
   <si>
     <t>Краткий отчет по товарам</t>
   </si>
@@ -710,6 +710,378 @@
   </si>
   <si>
     <t>Наволочка тенсель 50х70 - "Карибская волна"</t>
+  </si>
+  <si>
+    <t>4630460961793</t>
+  </si>
+  <si>
+    <t>Наволочка из тенселя 50 х 70 - М - Халкидики</t>
+  </si>
+  <si>
+    <t>4630460961786</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё полисатин Евро макси на резинке 180х200х30 - М - 80 - Витражи с наволочками 50х70</t>
+  </si>
+  <si>
+    <t>4630460961779</t>
+  </si>
+  <si>
+    <t>Простыня из сатина-жаккарда 240 х 260 - М - Палладион</t>
+  </si>
+  <si>
+    <t>4630460961762</t>
+  </si>
+  <si>
+    <t>Пододеяльник микросатин 240х260 - "Небосвод"</t>
+  </si>
+  <si>
+    <t>4630460961755</t>
+  </si>
+  <si>
+    <t>Простыня из тенселя 200 х 220 - М - Королевский пурпур</t>
+  </si>
+  <si>
+    <t>4630460961748</t>
+  </si>
+  <si>
+    <t>Пододеяльник из тенселя 200 х 220 - М - Пинклайт</t>
+  </si>
+  <si>
+    <t>4630460961731</t>
+  </si>
+  <si>
+    <t>Наволочка из тенселя 70 х 70 - М - Хрустальный оазис</t>
+  </si>
+  <si>
+    <t>4630460961724</t>
+  </si>
+  <si>
+    <t>Пододеяльник из тенселя 175 х 215 - М - Гималайские маки</t>
+  </si>
+  <si>
+    <t>4630460961717</t>
+  </si>
+  <si>
+    <t>Простыня микросатин 220х240 - "Метель"</t>
+  </si>
+  <si>
+    <t>4630460961700</t>
+  </si>
+  <si>
+    <t>Простыня круглая из тенселя на резинке 220х220х40 - М - 60S Белый</t>
+  </si>
+  <si>
+    <t>4630460961694</t>
+  </si>
+  <si>
+    <t>Пододеяльник из сатина 145х215 - "Небесный глянцевая"</t>
+  </si>
+  <si>
+    <t>4630460961687</t>
+  </si>
+  <si>
+    <t>Пододеяльник из сатина 145 х 215 - М - 125 - Голубая бирюза</t>
+  </si>
+  <si>
+    <t>4630460961670</t>
+  </si>
+  <si>
+    <t>Наволочка из сатина 50 х 70 - М - 130 - Ночная синева</t>
+  </si>
+  <si>
+    <t>4630460961663</t>
+  </si>
+  <si>
+    <t>Простыня Жатка 180х220 - "Парижский Шарм"</t>
+  </si>
+  <si>
+    <t>4630460961656</t>
+  </si>
+  <si>
+    <t>Пододеяльник твил-сатин 150 х 200 - "Дино-пати"</t>
+  </si>
+  <si>
+    <t>4630460961649</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё тенсель семейное на резинке 180х200х30 - М - 60S 129 Темно-зеленый с наволочками 50х70</t>
+  </si>
+  <si>
+    <t>4630460961632</t>
+  </si>
+  <si>
+    <t>Простыня из бязи на резинке 80 х 200 х 30 - М - 142 ГОСТ - Спящий Мишка на бежевом</t>
+  </si>
+  <si>
+    <t>4630460961625</t>
+  </si>
+  <si>
+    <t>Простыня из страйп-сатина 260 х 260 - М - 135 - Эмерэльд 1х1</t>
+  </si>
+  <si>
+    <t>4630460961618</t>
+  </si>
+  <si>
+    <t>Пододеяльник тенсель-жаккард 200 х 220 - "Табия"</t>
+  </si>
+  <si>
+    <t>4630460961601</t>
+  </si>
+  <si>
+    <t>Наволочка тенсель 50х70 - "Коньячный"</t>
+  </si>
+  <si>
+    <t>4630460961595</t>
+  </si>
+  <si>
+    <t>Наволочка тенсель 50х50 - "Коньячный"</t>
+  </si>
+  <si>
+    <t>4630460961588</t>
+  </si>
+  <si>
+    <t>Простыня Микрофибра 300х300 - "Эстрелья"</t>
+  </si>
+  <si>
+    <t>4630460961571</t>
+  </si>
+  <si>
+    <t>Простыня из страйп-сатина 280 х 280 - М - 135 - Белый 1х1</t>
+  </si>
+  <si>
+    <t>4630460961564</t>
+  </si>
+  <si>
+    <t>Наволочка Жатка 50х70 - "Снежный Хищник"</t>
+  </si>
+  <si>
+    <t>4630460961557</t>
+  </si>
+  <si>
+    <t>Наволочка из бязи 70 х 70 - М - 125 - Сансет</t>
+  </si>
+  <si>
+    <t>4630460961540</t>
+  </si>
+  <si>
+    <t>Простыня из сатина на резинке 200 х 200 х 40 - М - 125 - Голубая бирюза</t>
+  </si>
+  <si>
+    <t>4630460961533</t>
+  </si>
+  <si>
+    <t>Наволочка из тенселя 40 х 60 - М - 60S 4292 Кремовый</t>
+  </si>
+  <si>
+    <t>4630460961526</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё из страйп-сатина семейное на резинке 160х200х30 - М - 130 - Пел Догвуд 1х1</t>
+  </si>
+  <si>
+    <t>4630460961519</t>
+  </si>
+  <si>
+    <t>Простыня Жатка 300х300 - "Леопардовый Сон"</t>
+  </si>
+  <si>
+    <t>4630460961502</t>
+  </si>
+  <si>
+    <t>Пододеяльник Жатка 220х240 - "Леопардовый Сон"</t>
+  </si>
+  <si>
+    <t>4630460961496</t>
+  </si>
+  <si>
+    <t>Простыня из страйп-сатина на резинке 200 х 220 х 40 - М - 135 - Углерод 1х1</t>
+  </si>
+  <si>
+    <t>4630460961489</t>
+  </si>
+  <si>
+    <t>Простыня из страйп-сатина 240 х 260 - М - 125 - Шампань 3х3</t>
+  </si>
+  <si>
+    <t>4630460961472</t>
+  </si>
+  <si>
+    <t>Наволочка из сатина 50 х 70 - М - Изольда</t>
+  </si>
+  <si>
+    <t>4630460961465</t>
+  </si>
+  <si>
+    <t>Простыня микросатин 180х220 - "Легкий роман"</t>
+  </si>
+  <si>
+    <t>4630460961458</t>
+  </si>
+  <si>
+    <t>Простыня круглая из сатина на резинке 230 х 230 х 30 - М - 125 - Вишневые лепестки</t>
+  </si>
+  <si>
+    <t>4630460961441</t>
+  </si>
+  <si>
+    <t>Пододеяльник страйп-сатин 175х215 - 125 - "Миндаль" 1х1</t>
+  </si>
+  <si>
+    <t>4630460961434</t>
+  </si>
+  <si>
+    <t>Простыня круглая из перкаля на резинке 200 х 200 х 30 - М - 110 - Каори на зеленом</t>
+  </si>
+  <si>
+    <t>4630460961427</t>
+  </si>
+  <si>
+    <t>Пододеяльник из поплина 200 х 200 - М - Феста А+В</t>
+  </si>
+  <si>
+    <t>4630460961410</t>
+  </si>
+  <si>
+    <t>Наволочка из перкаля 70 х 70 - Р - М - Дуэт</t>
+  </si>
+  <si>
+    <t>4630460961403</t>
+  </si>
+  <si>
+    <t>Наволочка поплин 70 х 70 - "Оллорины"</t>
+  </si>
+  <si>
+    <t>4630460961397</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё тенсель-жаккард 2 спальное на резинке 160х200х30 - "Табия" с наволочками 50х70</t>
+  </si>
+  <si>
+    <t>4630460961380</t>
+  </si>
+  <si>
+    <t>Пододеяльник из страйп микрофибры 220 х 240 - М - 85 - Белый 3х3</t>
+  </si>
+  <si>
+    <t>4630460961373</t>
+  </si>
+  <si>
+    <t>Пододеяльник из сатина 200 х 220 - М - Красный</t>
+  </si>
+  <si>
+    <t>4630460961366</t>
+  </si>
+  <si>
+    <t>Наволочка тенсель 40 х 40 - "Белый Страйп"</t>
+  </si>
+  <si>
+    <t>4630460961359</t>
+  </si>
+  <si>
+    <t>КПБ Постельное белье тенсель 1,5 спальное - М - Черный блеск с наволочками 50х70</t>
+  </si>
+  <si>
+    <t>4630460961342</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё страйп-сатин Евро макси на резинке 180х200х30 - М - 135 - Марриотт Белый 3х3</t>
+  </si>
+  <si>
+    <t>4630460961335</t>
+  </si>
+  <si>
+    <t>Простыня из сатина 260 х 260 - М - 140 - Можиана Люкс</t>
+  </si>
+  <si>
+    <t>4630460961328</t>
+  </si>
+  <si>
+    <t>Простыня из перкаля на резинке 120 х 200 х 30 - М - 125 - Лунный песок</t>
+  </si>
+  <si>
+    <t>4630460961311</t>
+  </si>
+  <si>
+    <t>Простыня тенсель на резинке 200х220х20 - "Эрос"</t>
+  </si>
+  <si>
+    <t>4630460961304</t>
+  </si>
+  <si>
+    <t>Наволочка страйп-сатин 50х70 - 125 - "Индиго" 1х1</t>
+  </si>
+  <si>
+    <t>4630460961298</t>
+  </si>
+  <si>
+    <t>Пододеяльник варёный хлопок 200х220 - "Стальная тень" (меланж)</t>
+  </si>
+  <si>
+    <t>4630460961281</t>
+  </si>
+  <si>
+    <t>Простыня страйп-сатин на резинке 160х200х30 - 125 - "Олива" 1х1</t>
+  </si>
+  <si>
+    <t>4630460961274</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё тенсель Евро на резинке 160х200х30 - М - Блу Скай</t>
+  </si>
+  <si>
+    <t>4630460961267</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё полисатин семейное - "Глубь"</t>
+  </si>
+  <si>
+    <t>4630460961250</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё Жатка Евро на резинке 160х200х30 - "Замороженный Перец"</t>
+  </si>
+  <si>
+    <t>4630460961243</t>
+  </si>
+  <si>
+    <t>Простыня из поплина 220 х 240 - М - Гранола</t>
+  </si>
+  <si>
+    <t>4630460961236</t>
+  </si>
+  <si>
+    <t>Простыня полисатин 300х300 - "Синиль"</t>
+  </si>
+  <si>
+    <t>4630460961229</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё ранфорс 1,5 спальное на резинке 140х200х30 - "Фантасмагория" с наволочками 50х70</t>
+  </si>
+  <si>
+    <t>4630460961212</t>
+  </si>
+  <si>
+    <t>Простыня Жатка 180х220 - "Ромашковая Нежность"</t>
+  </si>
+  <si>
+    <t>4630460961205</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё перкаль Евро - М - 110 - Каори на зеленом с наволочками 50х70</t>
+  </si>
+  <si>
+    <t>4630460961199</t>
+  </si>
+  <si>
+    <t>Пододеяльник из тенселя 150 х 200 - М - Пинклайт</t>
+  </si>
+  <si>
+    <t>4630460961182</t>
+  </si>
+  <si>
+    <t>Пододеяльник тенсель 150 х 200 - "Серый Райнар"</t>
   </si>
 </sst>
 </file>
@@ -2019,6 +2391,502 @@
         <v>231</v>
       </c>
     </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>232</v>
+      </c>
+      <c r="B119" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>234</v>
+      </c>
+      <c r="B120" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>236</v>
+      </c>
+      <c r="B121" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>238</v>
+      </c>
+      <c r="B122" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>240</v>
+      </c>
+      <c r="B123" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>242</v>
+      </c>
+      <c r="B124" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>244</v>
+      </c>
+      <c r="B125" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
+        <v>246</v>
+      </c>
+      <c r="B126" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>248</v>
+      </c>
+      <c r="B127" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>250</v>
+      </c>
+      <c r="B128" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>252</v>
+      </c>
+      <c r="B129" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>254</v>
+      </c>
+      <c r="B130" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>256</v>
+      </c>
+      <c r="B131" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>258</v>
+      </c>
+      <c r="B132" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>260</v>
+      </c>
+      <c r="B133" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>262</v>
+      </c>
+      <c r="B134" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>264</v>
+      </c>
+      <c r="B135" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
+        <v>266</v>
+      </c>
+      <c r="B136" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>268</v>
+      </c>
+      <c r="B137" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>270</v>
+      </c>
+      <c r="B138" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>272</v>
+      </c>
+      <c r="B139" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>274</v>
+      </c>
+      <c r="B140" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>276</v>
+      </c>
+      <c r="B141" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A142" t="s">
+        <v>278</v>
+      </c>
+      <c r="B142" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>280</v>
+      </c>
+      <c r="B143" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A144" t="s">
+        <v>282</v>
+      </c>
+      <c r="B144" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>284</v>
+      </c>
+      <c r="B145" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>286</v>
+      </c>
+      <c r="B146" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>288</v>
+      </c>
+      <c r="B147" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A148" t="s">
+        <v>290</v>
+      </c>
+      <c r="B148" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>292</v>
+      </c>
+      <c r="B149" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A150" t="s">
+        <v>294</v>
+      </c>
+      <c r="B150" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>296</v>
+      </c>
+      <c r="B151" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>298</v>
+      </c>
+      <c r="B152" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>300</v>
+      </c>
+      <c r="B153" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>302</v>
+      </c>
+      <c r="B154" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>304</v>
+      </c>
+      <c r="B155" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>306</v>
+      </c>
+      <c r="B156" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>308</v>
+      </c>
+      <c r="B157" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>310</v>
+      </c>
+      <c r="B158" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>312</v>
+      </c>
+      <c r="B159" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>314</v>
+      </c>
+      <c r="B160" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>316</v>
+      </c>
+      <c r="B161" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>318</v>
+      </c>
+      <c r="B162" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>320</v>
+      </c>
+      <c r="B163" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>322</v>
+      </c>
+      <c r="B164" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>324</v>
+      </c>
+      <c r="B165" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>326</v>
+      </c>
+      <c r="B166" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>328</v>
+      </c>
+      <c r="B167" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>330</v>
+      </c>
+      <c r="B168" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>332</v>
+      </c>
+      <c r="B169" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>334</v>
+      </c>
+      <c r="B170" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>336</v>
+      </c>
+      <c r="B171" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>338</v>
+      </c>
+      <c r="B172" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>340</v>
+      </c>
+      <c r="B173" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>342</v>
+      </c>
+      <c r="B174" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>344</v>
+      </c>
+      <c r="B175" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>346</v>
+      </c>
+      <c r="B176" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>348</v>
+      </c>
+      <c r="B177" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>350</v>
+      </c>
+      <c r="B178" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>352</v>
+      </c>
+      <c r="B179" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>354</v>
+      </c>
+      <c r="B180" t="s">
+        <v>355</v>
+      </c>
+    </row>
     <row r="3449" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3449" s="5"/>
     </row>

</xml_diff>

<commit_message>
update short report & actual.html & endpoint /input_remarking
</commit_message>
<xml_diff>
--- a/public/Краткий отчет.xlsx
+++ b/public/Краткий отчет.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29628"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56AB988-C99D-46C6-9450-F2D37080A290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
-    <sheet name="Краткий отчет" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="Краткий отчет" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2798" uniqueCount="2798">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2902" uniqueCount="2902">
   <si>
     <t>Краткий отчет по товарам</t>
   </si>
@@ -8409,35 +8408,347 @@
   </si>
   <si>
     <t>КПБ Постельное белье микросатин 2 спальное на резинке 140х200х30 - "Страстный гранат"</t>
+  </si>
+  <si>
+    <t>4660674644472</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё поплин 2 спальное на резинке 140х200х30 - "Лазурный Мегаполис" с наволочками 50х70</t>
+  </si>
+  <si>
+    <t>4660674644465</t>
+  </si>
+  <si>
+    <t>Наволочка из бязи 70 х 70 - М - 142 - Сиреневые маки</t>
+  </si>
+  <si>
+    <t>4660674644458</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё тенсель 1,5 спальное - М - 60S Белый с наволочками 50х70</t>
+  </si>
+  <si>
+    <t>4660674644441</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё поплин 1,5 спальное на резинке 140х200х30 - М - Сливочно-кремовый</t>
+  </si>
+  <si>
+    <t>4660674644434</t>
+  </si>
+  <si>
+    <t>Простыня из бязи 150 х 220 - М - 142 ГОСТ - Оранжевый</t>
+  </si>
+  <si>
+    <t>4660674644427</t>
+  </si>
+  <si>
+    <t>Пододеяльник из тенселя 150 х 200 - М - Горький шоколад</t>
+  </si>
+  <si>
+    <t>4660674644410</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё полисатин семейное на резинке 160х200х30 - "Зайга"</t>
+  </si>
+  <si>
+    <t>4660674644403</t>
+  </si>
+  <si>
+    <t>Простыня полисатин на резинке 200х200х40 - "Олуфими"</t>
+  </si>
+  <si>
+    <t>4660674644397</t>
+  </si>
+  <si>
+    <t>Наволочка из тенселя 50 х 70 - М - 60S 4307 Сливочный Страйп 1х1</t>
+  </si>
+  <si>
+    <t>4660674644380</t>
+  </si>
+  <si>
+    <t>Простыня из страйп-сатина 280 х 280 - М - 125 - Дымка 1х1</t>
+  </si>
+  <si>
+    <t>4660674644373</t>
+  </si>
+  <si>
+    <t>Простыня полисатин на резинке 180х200х40 - "Аврела"</t>
+  </si>
+  <si>
+    <t>4660674644366</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё Жатка 1,5 спальное на резинке 120х200х30 - "Бирюзовый Рельеф" с наволочками 50х70</t>
+  </si>
+  <si>
+    <t>4660674644359</t>
+  </si>
+  <si>
+    <t>Простыня из тенселя на резинке 180х200х40 - М - 60S 129 Темно-зеленый</t>
+  </si>
+  <si>
+    <t>4660674644342</t>
+  </si>
+  <si>
+    <t>Простыня из тенселя 180 х 220 - М - 60S 4225 Зелёный лесной</t>
+  </si>
+  <si>
+    <t>4660674644335</t>
+  </si>
+  <si>
+    <t>Простыня из сатина на резинке 180 х 200 х 40 - М - 125 - Капучино</t>
+  </si>
+  <si>
+    <t>4660674644328</t>
+  </si>
+  <si>
+    <t>Простыня из страйп-сатина 300 х 300 - М - 125 - Шампань 3х3</t>
+  </si>
+  <si>
+    <t>4660674644311</t>
+  </si>
+  <si>
+    <t>Пододеяльник твил-сатин 150 х 200 - "Лесная тень"</t>
+  </si>
+  <si>
+    <t>4660674644304</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё сатин Браш 1,5 спальное на резинке 140х200х30 - М - Кремовый бархат</t>
+  </si>
+  <si>
+    <t>4660674644298</t>
+  </si>
+  <si>
+    <t>КПБ Постельное белье тенсель 2 спальное с Евро простыней - "Карибская волна"</t>
+  </si>
+  <si>
+    <t>4660674644281</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё поплин семейное - М - Прелат А+В с наволочками 50х70</t>
+  </si>
+  <si>
+    <t>4660674644274</t>
+  </si>
+  <si>
+    <t>Простыня полисатин 300х300 - "Мелиссит"</t>
+  </si>
+  <si>
+    <t>4660674644267</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё перкаль 1,5 спальное на резинке 90х200х30 - М - 125 - Дождевая туча с наволочками 50х70</t>
+  </si>
+  <si>
+    <t>4660674644250</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё Жатка 2 спальное с Евро простыней - "Звёздный туман"</t>
+  </si>
+  <si>
+    <t>4660674644243</t>
+  </si>
+  <si>
+    <t>Наволочка из бязи 70 х 70 - М - 142 - Плата</t>
+  </si>
+  <si>
+    <t>4660674644236</t>
+  </si>
+  <si>
+    <t>Пододеяльник твил-сатин 220 х 240 - "Ламы"</t>
+  </si>
+  <si>
+    <t>4660674644229</t>
+  </si>
+  <si>
+    <t>Простыня тенсель 200х220 - "Чёрный Страйп"</t>
+  </si>
+  <si>
+    <t>4660674644212</t>
+  </si>
+  <si>
+    <t>Наволочка из тенселя 70 х 70 - М - 60S 22 Светло-розовый</t>
+  </si>
+  <si>
+    <t>4660674644205</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё поплин 2 спальное - "Корги-пати"</t>
+  </si>
+  <si>
+    <t>4660674644199</t>
+  </si>
+  <si>
+    <t>Пододеяльник из страйп сатина 150х200 - 130 - "Изумрудный малахит" 1х1</t>
+  </si>
+  <si>
+    <t>4660674644182</t>
+  </si>
+  <si>
+    <t>Простыня страйп-сатин 280х280 - "Дюмар" 1х1</t>
+  </si>
+  <si>
+    <t>4660674644175</t>
+  </si>
+  <si>
+    <t>Простыня страйп-сатин 280х280 - "Калинте" 1х1</t>
+  </si>
+  <si>
+    <t>4660674644168</t>
+  </si>
+  <si>
+    <t>Наволочка из тенселя 50 х 70 - М - Черный блеск</t>
+  </si>
+  <si>
+    <t>4660674644151</t>
+  </si>
+  <si>
+    <t>Пододеяльник твил-сатин 150 х 200 - "Ламы"</t>
+  </si>
+  <si>
+    <t>4660674644144</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё перкаль Евро макси - М - 125 - Дождевая туча с наволочками 50х70</t>
+  </si>
+  <si>
+    <t>4660674644137</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё бязь 1,5 спальное - М - 120 - Голубая Латка</t>
+  </si>
+  <si>
+    <t>4660674644120</t>
+  </si>
+  <si>
+    <t>Простыня полисатин 280х280 - "Линнея"</t>
+  </si>
+  <si>
+    <t>4660674644113</t>
+  </si>
+  <si>
+    <t>Простыня полисатин 280х280 - "Глисса"</t>
+  </si>
+  <si>
+    <t>4660674644106</t>
+  </si>
+  <si>
+    <t>Простыня полисатин 280х280 - "Глубь"</t>
+  </si>
+  <si>
+    <t>4660674644090</t>
+  </si>
+  <si>
+    <t>Пододеяльник микросатин 220х240 - "Легкий роман"</t>
+  </si>
+  <si>
+    <t>4660674644083</t>
+  </si>
+  <si>
+    <t>Простыня полисатин 280х280 - "Эвергрин"</t>
+  </si>
+  <si>
+    <t>4660674644076</t>
+  </si>
+  <si>
+    <t>Простыня микросатин 280х280 - "Легкий роман"</t>
+  </si>
+  <si>
+    <t>4660674644069</t>
+  </si>
+  <si>
+    <t>Пододеяльник микросатин 220х240 - "Страстный гранат"</t>
+  </si>
+  <si>
+    <t>4660674644052</t>
+  </si>
+  <si>
+    <t>Пододеяльник из поплина 150 х 200 - "Астролябия" А+В</t>
+  </si>
+  <si>
+    <t>4660674644045</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё сатин 1,5 спальное на резинке 120х200х30 - М - Сарсуэла с наволочками 50х70</t>
+  </si>
+  <si>
+    <t>4660674644038</t>
+  </si>
+  <si>
+    <t>Наволочка из варёного хлопка 50 х 70 - М - Чёрная гавань</t>
+  </si>
+  <si>
+    <t>4660674644021</t>
+  </si>
+  <si>
+    <t>Наволочка из тенселя 70 х 70 - М - Горчица</t>
+  </si>
+  <si>
+    <t>4660674644489</t>
+  </si>
+  <si>
+    <t>Простыня Жатка на резинке 160х200х40 - "Лесная Мелодия"</t>
+  </si>
+  <si>
+    <t>4660674644526</t>
+  </si>
+  <si>
+    <t>Простыня из тенселя на резинке 180х200х30 - М - Королевский пурпур</t>
+  </si>
+  <si>
+    <t>4660674644519</t>
+  </si>
+  <si>
+    <t>Пододеяльник поплин 200х220 - "Лериса"</t>
+  </si>
+  <si>
+    <t>4660674644502</t>
+  </si>
+  <si>
+    <t>Простыня из поплина 220 х 240 - М - В ассортименте</t>
+  </si>
+  <si>
+    <t>4660674644496</t>
+  </si>
+  <si>
+    <t>Наволочка поплин 40х60 - "Ягуар"</t>
+  </si>
+  <si>
+    <t>4660674644533</t>
+  </si>
+  <si>
+    <t>Простыня из креп-жатки 180 х 220 - М - 80 - Теплые Пожелания</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
+      <charset val="1"/>
+      <family val="2"/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
+      <charset val="1"/>
+      <family val="2"/>
       <sz val="10"/>
       <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -8463,18 +8774,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -8498,7 +8801,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -8775,26 +9078,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P11478"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:P11478"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1366" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A1377" sqref="A1377:B1401"/>
+    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
+      <selection activeCell="A1377" sqref="A1377"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="177" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -8821,7 +9124,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -8829,7 +9132,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -8837,7 +9140,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -8845,7 +9148,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -8853,7 +9156,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -8861,7 +9164,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -8869,7 +9172,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -8877,7 +9180,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -8885,7 +9188,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -8893,7 +9196,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -8901,7 +9204,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -8909,7 +9212,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -19997,13 +20300,429 @@
         <v>2797</v>
       </c>
     </row>
+    <row r="1402" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1402" t="s">
+        <v>2798</v>
+      </c>
+      <c r="B1402" t="s">
+        <v>2799</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1403" t="s">
+        <v>2800</v>
+      </c>
+      <c r="B1403" t="s">
+        <v>2801</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1404" t="s">
+        <v>2802</v>
+      </c>
+      <c r="B1404" t="s">
+        <v>2803</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1405" t="s">
+        <v>2804</v>
+      </c>
+      <c r="B1405" t="s">
+        <v>2805</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1406" t="s">
+        <v>2806</v>
+      </c>
+      <c r="B1406" t="s">
+        <v>2807</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1407" t="s">
+        <v>2808</v>
+      </c>
+      <c r="B1407" t="s">
+        <v>2809</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1408" t="s">
+        <v>2810</v>
+      </c>
+      <c r="B1408" t="s">
+        <v>2811</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1409" t="s">
+        <v>2812</v>
+      </c>
+      <c r="B1409" t="s">
+        <v>2813</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1410" t="s">
+        <v>2814</v>
+      </c>
+      <c r="B1410" t="s">
+        <v>2815</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1411" t="s">
+        <v>2816</v>
+      </c>
+      <c r="B1411" t="s">
+        <v>2817</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1412" t="s">
+        <v>2818</v>
+      </c>
+      <c r="B1412" t="s">
+        <v>2819</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1413" t="s">
+        <v>2820</v>
+      </c>
+      <c r="B1413" t="s">
+        <v>2821</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1414" t="s">
+        <v>2822</v>
+      </c>
+      <c r="B1414" t="s">
+        <v>2823</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1415" t="s">
+        <v>2824</v>
+      </c>
+      <c r="B1415" t="s">
+        <v>2825</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1416" t="s">
+        <v>2826</v>
+      </c>
+      <c r="B1416" t="s">
+        <v>2827</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1417" t="s">
+        <v>2828</v>
+      </c>
+      <c r="B1417" t="s">
+        <v>2829</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1418" t="s">
+        <v>2830</v>
+      </c>
+      <c r="B1418" t="s">
+        <v>2831</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1419" t="s">
+        <v>2832</v>
+      </c>
+      <c r="B1419" t="s">
+        <v>2833</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1420" t="s">
+        <v>2834</v>
+      </c>
+      <c r="B1420" t="s">
+        <v>2835</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1421" t="s">
+        <v>2836</v>
+      </c>
+      <c r="B1421" t="s">
+        <v>2837</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1422" t="s">
+        <v>2838</v>
+      </c>
+      <c r="B1422" t="s">
+        <v>2839</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1423" t="s">
+        <v>2840</v>
+      </c>
+      <c r="B1423" t="s">
+        <v>2841</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1424" t="s">
+        <v>2842</v>
+      </c>
+      <c r="B1424" t="s">
+        <v>2843</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1425" t="s">
+        <v>2844</v>
+      </c>
+      <c r="B1425" t="s">
+        <v>2845</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1426" t="s">
+        <v>2846</v>
+      </c>
+      <c r="B1426" t="s">
+        <v>2847</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1427" t="s">
+        <v>2848</v>
+      </c>
+      <c r="B1427" t="s">
+        <v>2849</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1428" t="s">
+        <v>2850</v>
+      </c>
+      <c r="B1428" t="s">
+        <v>2851</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1429" t="s">
+        <v>2852</v>
+      </c>
+      <c r="B1429" t="s">
+        <v>2853</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1430" t="s">
+        <v>2854</v>
+      </c>
+      <c r="B1430" t="s">
+        <v>2855</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1431" t="s">
+        <v>2856</v>
+      </c>
+      <c r="B1431" t="s">
+        <v>2857</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1432" t="s">
+        <v>2858</v>
+      </c>
+      <c r="B1432" t="s">
+        <v>2859</v>
+      </c>
+    </row>
+    <row r="1433" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1433" t="s">
+        <v>2860</v>
+      </c>
+      <c r="B1433" t="s">
+        <v>2861</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1434" t="s">
+        <v>2862</v>
+      </c>
+      <c r="B1434" t="s">
+        <v>2863</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1435" t="s">
+        <v>2864</v>
+      </c>
+      <c r="B1435" t="s">
+        <v>2865</v>
+      </c>
+    </row>
+    <row r="1436" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1436" t="s">
+        <v>2866</v>
+      </c>
+      <c r="B1436" t="s">
+        <v>2867</v>
+      </c>
+    </row>
+    <row r="1437" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1437" t="s">
+        <v>2868</v>
+      </c>
+      <c r="B1437" t="s">
+        <v>2869</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1438" t="s">
+        <v>2870</v>
+      </c>
+      <c r="B1438" t="s">
+        <v>2871</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1439" t="s">
+        <v>2872</v>
+      </c>
+      <c r="B1439" t="s">
+        <v>2873</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1440" t="s">
+        <v>2874</v>
+      </c>
+      <c r="B1440" t="s">
+        <v>2875</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1441" t="s">
+        <v>2876</v>
+      </c>
+      <c r="B1441" t="s">
+        <v>2877</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1442" t="s">
+        <v>2878</v>
+      </c>
+      <c r="B1442" t="s">
+        <v>2879</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1443" t="s">
+        <v>2880</v>
+      </c>
+      <c r="B1443" t="s">
+        <v>2881</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1444" t="s">
+        <v>2882</v>
+      </c>
+      <c r="B1444" t="s">
+        <v>2883</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1445" t="s">
+        <v>2884</v>
+      </c>
+      <c r="B1445" t="s">
+        <v>2885</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1446" t="s">
+        <v>2886</v>
+      </c>
+      <c r="B1446" t="s">
+        <v>2887</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1447" t="s">
+        <v>2888</v>
+      </c>
+      <c r="B1447" t="s">
+        <v>2889</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1448" t="s">
+        <v>2890</v>
+      </c>
+      <c r="B1448" t="s">
+        <v>2891</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1449" t="s">
+        <v>2892</v>
+      </c>
+      <c r="B1449" t="s">
+        <v>2893</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1450" t="s">
+        <v>2894</v>
+      </c>
+      <c r="B1450" t="s">
+        <v>2895</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1451" t="s">
+        <v>2896</v>
+      </c>
+      <c r="B1451" t="s">
+        <v>2897</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1452" t="s">
+        <v>2898</v>
+      </c>
+      <c r="B1452" t="s">
+        <v>2899</v>
+      </c>
+    </row>
+    <row r="1453" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1453" t="s">
+        <v>2900</v>
+      </c>
+      <c r="B1453" t="s">
+        <v>2901</v>
+      </c>
+    </row>
     <row r="3449" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3449" s="6"/>
     </row>
     <row r="4853" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4853" s="7"/>
     </row>
-    <row r="4890" spans="7:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4890" ht="26.25" customHeight="1" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G4890" s="7"/>
     </row>
     <row r="7716" spans="2:2" x14ac:dyDescent="0.25">
@@ -20019,6 +20738,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update actual_marks; short_report; /test_features endpoint
</commit_message>
<xml_diff>
--- a/public/Краткий отчет.xlsx
+++ b/public/Краткий отчет.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29628"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9DCFECC-92D5-4BE1-A88A-2FC2219BD5B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet sheetId="1" name="Краткий отчет" state="visible" r:id="rId4"/>
+    <sheet name="Краткий отчет" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2966" uniqueCount="2966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3003" uniqueCount="3003">
   <si>
     <t>Краткий отчет по товарам</t>
   </si>
@@ -8912,35 +8913,146 @@
   </si>
   <si>
     <t>Пододеяльник страйп-сатин 200х220 - 125 - "Крем" 1х1</t>
+  </si>
+  <si>
+    <t>4660674645011</t>
+  </si>
+  <si>
+    <t>КПБ Постельное бельё страйп-сатин 1,5 спальное - М - 140 - Росток 1х1 Универсал</t>
+  </si>
+  <si>
+    <t>4660674645004</t>
+  </si>
+  <si>
+    <t>Простыня круглая из страйп сатина на резинке 200 x 200 х 20 - М - 130 - Серый туман 1х1</t>
+  </si>
+  <si>
+    <t>4660674644991</t>
+  </si>
+  <si>
+    <t>Простыня из сатина 220 х 240 - М - 120 - В ассортименте</t>
+  </si>
+  <si>
+    <t>4660674644984</t>
+  </si>
+  <si>
+    <t>КПБ Детское постельное бельё бязь 1,5 спальное - М - 120 - Колыбель на зеленом</t>
+  </si>
+  <si>
+    <t>4660674644977</t>
+  </si>
+  <si>
+    <t>Пододеяльник микросатин 220х240 - "Смоки"</t>
+  </si>
+  <si>
+    <t>4660674644960</t>
+  </si>
+  <si>
+    <t>Наволочка из страйп-сатина 50 х 50 - М - 130 - Мятный фреш 1х1</t>
+  </si>
+  <si>
+    <t>4660674644953</t>
+  </si>
+  <si>
+    <t>Простыня страйп-сатин на резинке 160х200х40 - 125 - "Серебро" 1х1</t>
+  </si>
+  <si>
+    <t>4660674644946</t>
+  </si>
+  <si>
+    <t>Простыня тенсель на резинке 160х200х30 - М - Морской</t>
+  </si>
+  <si>
+    <t>4660674644939</t>
+  </si>
+  <si>
+    <t>Наволочка Жатка 70х70 - "Бирюзовый Рельеф"</t>
+  </si>
+  <si>
+    <t>4660674644922</t>
+  </si>
+  <si>
+    <t>Пододеяльник Жатка 200х200 - "Бирюзовый Рельеф"</t>
+  </si>
+  <si>
+    <t>4660674644915</t>
+  </si>
+  <si>
+    <t>Простыня Жатка на резинке 160х200х20 - "Бирюзовый Рельеф"</t>
+  </si>
+  <si>
+    <t>4660674644908</t>
+  </si>
+  <si>
+    <t>Наволочка из варёного хлопка 50 х 70 - М - Серо-зелёный</t>
+  </si>
+  <si>
+    <t>4660674644892</t>
+  </si>
+  <si>
+    <t>Наволочка ранфорс 50х70 - "Фантасмагория"</t>
+  </si>
+  <si>
+    <t>4660674644885</t>
+  </si>
+  <si>
+    <t>Простыня круглая микросатин на резинке 200х200х20 - "Шторм"</t>
+  </si>
+  <si>
+    <t>4660674644878</t>
+  </si>
+  <si>
+    <t>Простыня круглая микросатин на резинке 200х200х20 - "Бездна"</t>
+  </si>
+  <si>
+    <t>4660674644861</t>
+  </si>
+  <si>
+    <t>Пододеяльник полисатин 200х200 - "Эдже"</t>
+  </si>
+  <si>
+    <t>4660674645035</t>
+  </si>
+  <si>
+    <t>Наволочка тенсель 70х70 - "Розовый Флёр"</t>
+  </si>
+  <si>
+    <t>4660674645028</t>
+  </si>
+  <si>
+    <t>Пододеяльник страйп-сатин 200х200 - "Гриновей" 1х1</t>
+  </si>
+  <si>
+    <t>Дата создания</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-      <sz val="11"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <charset val="1"/>
-      <family val="2"/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
-      <charset val="1"/>
-      <family val="2"/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -8966,10 +9078,18 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -8993,7 +9113,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -9270,26 +9390,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P11478"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P11478"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" zoomScaleNormal="100">
-      <selection activeCell="A1377" sqref="A1377"/>
+    <sheetView tabSelected="1" topLeftCell="A1483" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C1504" sqref="A1504:C1505"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" customWidth="1"/>
     <col min="2" max="2" width="177" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -9301,7 +9422,9 @@
       <c r="B4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="3" t="s">
+        <v>3002</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
@@ -9316,7 +9439,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -9324,7 +9447,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -9332,7 +9455,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -9340,7 +9463,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -9348,7 +9471,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -9356,7 +9479,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -9364,7 +9487,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>16</v>
       </c>
@@ -9372,7 +9495,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -9380,7 +9503,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -9388,7 +9511,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -9396,7 +9519,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -9404,7 +9527,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -21164,13 +21287,157 @@
         <v>2965</v>
       </c>
     </row>
+    <row r="1486" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1486" t="s">
+        <v>2966</v>
+      </c>
+      <c r="B1486" t="s">
+        <v>2967</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1487" t="s">
+        <v>2968</v>
+      </c>
+      <c r="B1487" t="s">
+        <v>2969</v>
+      </c>
+    </row>
+    <row r="1488" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1488" t="s">
+        <v>2970</v>
+      </c>
+      <c r="B1488" t="s">
+        <v>2971</v>
+      </c>
+    </row>
+    <row r="1489" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1489" t="s">
+        <v>2972</v>
+      </c>
+      <c r="B1489" t="s">
+        <v>2973</v>
+      </c>
+    </row>
+    <row r="1490" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1490" t="s">
+        <v>2974</v>
+      </c>
+      <c r="B1490" t="s">
+        <v>2975</v>
+      </c>
+    </row>
+    <row r="1491" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1491" t="s">
+        <v>2976</v>
+      </c>
+      <c r="B1491" t="s">
+        <v>2977</v>
+      </c>
+    </row>
+    <row r="1492" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1492" t="s">
+        <v>2978</v>
+      </c>
+      <c r="B1492" t="s">
+        <v>2979</v>
+      </c>
+    </row>
+    <row r="1493" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1493" t="s">
+        <v>2980</v>
+      </c>
+      <c r="B1493" t="s">
+        <v>2981</v>
+      </c>
+    </row>
+    <row r="1494" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1494" t="s">
+        <v>2982</v>
+      </c>
+      <c r="B1494" t="s">
+        <v>2983</v>
+      </c>
+    </row>
+    <row r="1495" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1495" t="s">
+        <v>2984</v>
+      </c>
+      <c r="B1495" t="s">
+        <v>2985</v>
+      </c>
+    </row>
+    <row r="1496" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1496" t="s">
+        <v>2986</v>
+      </c>
+      <c r="B1496" t="s">
+        <v>2987</v>
+      </c>
+    </row>
+    <row r="1497" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1497" t="s">
+        <v>2988</v>
+      </c>
+      <c r="B1497" t="s">
+        <v>2989</v>
+      </c>
+    </row>
+    <row r="1498" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1498" t="s">
+        <v>2990</v>
+      </c>
+      <c r="B1498" t="s">
+        <v>2991</v>
+      </c>
+    </row>
+    <row r="1499" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1499" t="s">
+        <v>2992</v>
+      </c>
+      <c r="B1499" t="s">
+        <v>2993</v>
+      </c>
+    </row>
+    <row r="1500" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1500" t="s">
+        <v>2994</v>
+      </c>
+      <c r="B1500" t="s">
+        <v>2995</v>
+      </c>
+    </row>
+    <row r="1501" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1501" t="s">
+        <v>2996</v>
+      </c>
+      <c r="B1501" t="s">
+        <v>2997</v>
+      </c>
+    </row>
+    <row r="1502" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1502" t="s">
+        <v>2998</v>
+      </c>
+      <c r="B1502" t="s">
+        <v>2999</v>
+      </c>
+    </row>
+    <row r="1503" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1503" t="s">
+        <v>3000</v>
+      </c>
+      <c r="B1503" t="s">
+        <v>3001</v>
+      </c>
+    </row>
     <row r="3449" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3449" s="6"/>
     </row>
     <row r="4853" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4853" s="7"/>
     </row>
-    <row r="4890" ht="26.25" customHeight="1" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="4890" spans="7:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G4890" s="7"/>
     </row>
     <row r="7716" spans="2:2" x14ac:dyDescent="0.25">
@@ -21186,6 +21453,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967295" verticalDpi="4294967295"/>
 </worksheet>
 </file>
</xml_diff>